<commit_message>
opdateret tid på rapport
</commit_message>
<xml_diff>
--- a/Til burndown.xlsx
+++ b/Til burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\GitHub\DDU-Eksamensprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147284B2-911D-4F84-BD43-8D98142C8349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0169C0D-77E0-499E-9BC0-5C3A9979D29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -747,7 +747,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -847,24 +847,35 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44656</v>
+      </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>100.2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C6" s="1"/>
+      <c r="B6">
+        <v>2.25</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44656</v>
+      </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -875,7 +886,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -885,7 +896,7 @@
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -895,7 +906,7 @@
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -905,7 +916,7 @@
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -915,7 +926,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -925,7 +936,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -935,7 +946,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -945,7 +956,7 @@
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -955,7 +966,7 @@
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -965,7 +976,7 @@
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="17" spans="11:12" x14ac:dyDescent="0.35">
@@ -975,7 +986,7 @@
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="18" spans="11:12" x14ac:dyDescent="0.35">
@@ -985,7 +996,7 @@
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="19" spans="11:12" x14ac:dyDescent="0.35">
@@ -995,7 +1006,7 @@
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="20" spans="11:12" x14ac:dyDescent="0.35">
@@ -1005,7 +1016,7 @@
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="21" spans="11:12" x14ac:dyDescent="0.35">
@@ -1015,7 +1026,7 @@
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="22" spans="11:12" x14ac:dyDescent="0.35">
@@ -1025,7 +1036,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="23" spans="11:12" x14ac:dyDescent="0.35">
@@ -1035,7 +1046,7 @@
       </c>
       <c r="L23">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="24" spans="11:12" x14ac:dyDescent="0.35">
@@ -1045,7 +1056,7 @@
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="25" spans="11:12" x14ac:dyDescent="0.35">
@@ -1055,7 +1066,7 @@
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="26" spans="11:12" x14ac:dyDescent="0.35">
@@ -1065,7 +1076,7 @@
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>102.25</v>
+        <v>97.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daniell dit burndown er fuckd
</commit_message>
<xml_diff>
--- a/Til burndown.xlsx
+++ b/Til burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef72ee1a1b1c74f8/Documents/GitHub/DDU-Eksamensprojekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clara Maj\Documents\GitHub\DDU-Eksamensprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{F96EFBFD-B3D5-4EE0-AAC2-F9212016E5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A6CDA78-F9BB-4F8A-ABEB-7A7EA94F03A0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645BCCCD-D365-472C-ACE2-2EF7B9512DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5625" yWindow="3758" windowWidth="16875" windowHeight="10522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>Størrelse af task (t)</t>
   </si>
@@ -184,6 +184,42 @@
   </si>
   <si>
     <t>Database indkøbskurv</t>
+  </si>
+  <si>
+    <t>Indkøbskurv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Check ud </t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Vare information</t>
+  </si>
+  <si>
+    <t>Database wallet</t>
+  </si>
+  <si>
+    <t>Database check ud</t>
+  </si>
+  <si>
+    <t>Opret kort</t>
+  </si>
+  <si>
+    <t>Gemte kurv</t>
+  </si>
+  <si>
+    <t>Database gemte kurv</t>
+  </si>
+  <si>
+    <t>Check ud</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>Dataindsættelse indkøbskurv</t>
   </si>
 </sst>
 </file>
@@ -516,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="G49" workbookViewId="0">
+      <selection activeCell="M59" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1260,11 +1296,11 @@
         <v>44690</v>
       </c>
       <c r="K38">
-        <f t="shared" ref="K38:K50" si="7">IF(C38&lt;&gt;0,DAYS360($F$1,C38),0)</f>
+        <f t="shared" ref="K38:K65" si="7">IF(C38&lt;&gt;0,DAYS360($F$1,C38),0)</f>
         <v>47</v>
       </c>
       <c r="L38">
-        <f t="shared" ref="L38:L50" si="8">L37-B38</f>
+        <f t="shared" ref="L38:L65" si="8">L37-B38</f>
         <v>92.79</v>
       </c>
     </row>
@@ -1478,13 +1514,307 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
+        <v>44692</v>
+      </c>
       <c r="K50">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="L50">
         <f t="shared" si="8"/>
         <v>61.87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>0.25</v>
+      </c>
+      <c r="C51" s="1">
+        <v>44692</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="8"/>
+        <v>61.62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52" s="1">
+        <v>44692</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="8"/>
+        <v>55.62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C53" s="1">
+        <v>44692</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="8"/>
+        <v>55.07</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="C54" s="1">
+        <v>44692</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="7"/>
+        <v>49</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="8"/>
+        <v>53.02</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
+        <v>44693</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="8"/>
+        <v>53.02</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>0.26</v>
+      </c>
+      <c r="C56" s="1">
+        <v>44693</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="8"/>
+        <v>52.760000000000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>0.6</v>
+      </c>
+      <c r="C57" s="1">
+        <v>44693</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="8"/>
+        <v>52.160000000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>0.16</v>
+      </c>
+      <c r="C58" s="1">
+        <v>44693</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="8"/>
+        <v>52.000000000000007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1">
+        <v>44694</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="8"/>
+        <v>52.000000000000007</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>0.26</v>
+      </c>
+      <c r="C60" s="1">
+        <v>44694</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="8"/>
+        <v>51.740000000000009</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>0.26</v>
+      </c>
+      <c r="C61" s="1">
+        <v>44694</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="8"/>
+        <v>51.480000000000011</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>0.6</v>
+      </c>
+      <c r="C62" s="1">
+        <v>44694</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="8"/>
+        <v>50.88000000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>0.6</v>
+      </c>
+      <c r="C63" s="1">
+        <v>44694</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="8"/>
+        <v>50.280000000000008</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64" s="1">
+        <v>44695</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="8"/>
+        <v>50.280000000000008</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B65">
+        <v>20.6</v>
+      </c>
+      <c r="C65" s="1">
+        <v>44695</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="8"/>
+        <v>29.680000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>